<commit_message>
ver 0.1 first time, works on star helios 2017-8-8 file
</commit_message>
<xml_diff>
--- a/samples/InvestmentCodeLookup.xlsx
+++ b/samples/InvestmentCodeLookup.xlsx
@@ -16,179 +16,336 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentManualCount="8"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t>CITI code</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
+    <t>XS1464929329</t>
+  </si>
+  <si>
+    <t>BD1FF76</t>
+  </si>
+  <si>
+    <t>BDF16K0</t>
+  </si>
+  <si>
+    <t>XS1422790615</t>
+  </si>
+  <si>
+    <t>XS1565684062</t>
+  </si>
+  <si>
+    <t>BYQCMB2</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>ISIN/Geneva</t>
+  </si>
+  <si>
+    <t>BF0M6J1</t>
+  </si>
+  <si>
+    <t>AMBER TREASURE NANHAI 3 05/25/20</t>
+  </si>
+  <si>
+    <t>XS1619006643</t>
+  </si>
+  <si>
+    <t>BDRJQ79</t>
+  </si>
+  <si>
+    <t>AOYUAN PROPERTY CAPG 6.35 01/11/20</t>
+  </si>
+  <si>
+    <t>XS1543555533</t>
+  </si>
+  <si>
+    <t>BD1R420</t>
+  </si>
+  <si>
+    <t>BANK OF EAST ASIA LTD FRN 29DEC2049</t>
+  </si>
+  <si>
+    <t>XS1615078141</t>
+  </si>
+  <si>
+    <t>BYMJ7Y5</t>
+  </si>
+  <si>
+    <t>BAOXIN AUTO FIN CHGRAU 8 3/4 12/29/49</t>
+  </si>
+  <si>
+    <t>XS1519630484</t>
+  </si>
+  <si>
+    <t>BYMPWV5</t>
+  </si>
+  <si>
+    <t>BRIGHT GALAXY INTL LTD 3.375% 03NOV2021</t>
+  </si>
+  <si>
+    <t>XS1508782098</t>
+  </si>
+  <si>
+    <t>BY46HF5</t>
+  </si>
+  <si>
+    <t>CHINA AOYUAN PRO CAPG 10 7/8 05/26/18</t>
+  </si>
+  <si>
+    <t>XS1221908897</t>
+  </si>
+  <si>
+    <t>BF08G22</t>
+  </si>
+  <si>
+    <t>CHINA CINDA 2017 CCAMCL 3 03/09/20</t>
+  </si>
+  <si>
+    <t>XS1573134878</t>
+  </si>
+  <si>
+    <t>BF088D7</t>
+  </si>
+  <si>
+    <t>CHINA CINDA 2017 CCAMCL 3.65 03/09/22</t>
+  </si>
+  <si>
+    <t>XS1573134522</t>
+  </si>
+  <si>
+    <t>BD3DTW1</t>
+  </si>
+  <si>
+    <t>CHINA EVERGRANDE EVERRE 8 1/4 03/23/22</t>
+  </si>
+  <si>
+    <t>XS1580431143</t>
+  </si>
+  <si>
+    <t>BS7K2C4</t>
+  </si>
+  <si>
+    <t>CHINA HONGQIAO HONGQI 6 7/8 05/03/18</t>
+  </si>
+  <si>
+    <t>XS1132125946</t>
+  </si>
+  <si>
+    <t>BYW7448</t>
+  </si>
+  <si>
+    <t>CHINA SCE PROPER CHINSC 10 07/02/20</t>
+  </si>
+  <si>
+    <t>XS1241497384</t>
+  </si>
+  <si>
+    <t>BYP7887</t>
+  </si>
+  <si>
+    <t>CITIGROUP INC C 0 05/17/24</t>
+  </si>
+  <si>
+    <t>US172967LL34</t>
+  </si>
+  <si>
+    <t>BF3WL04</t>
+  </si>
+  <si>
+    <t>CK HUTCHISON CAPITAL FRN 31DEC2049</t>
+  </si>
+  <si>
+    <t>USG2176GAA97</t>
+  </si>
+  <si>
+    <t>BYZ6CP9</t>
+  </si>
+  <si>
+    <t>CNAC HK FINBRIDGE CO LTD 3% 19JUL2020</t>
+  </si>
+  <si>
+    <t>XS1644428614</t>
+  </si>
+  <si>
+    <t>B976111</t>
+  </si>
+  <si>
+    <t>COUNTRY GARDEN COGARD 7 1/2 01/10/23</t>
+  </si>
+  <si>
+    <t>USG24524AG84</t>
+  </si>
+  <si>
+    <t>BW40Q78</t>
+  </si>
+  <si>
+    <t>COUNTRY GARDEN COGARD 7 1/2 03/09/20</t>
+  </si>
+  <si>
+    <t>XS1164776020</t>
+  </si>
+  <si>
+    <t>BCRW3Z8</t>
+  </si>
+  <si>
+    <t>COUNTRY GARDEN COGARD 7 1/4 04/04/21</t>
+  </si>
+  <si>
+    <t>USG24524AH67</t>
+  </si>
+  <si>
+    <t>BYV3W87</t>
+  </si>
+  <si>
+    <t>DEMETER (SWISS RE LTD) FRN 31DEC2049</t>
+  </si>
+  <si>
+    <t>XS1640851983</t>
+  </si>
+  <si>
+    <t>BF29XP5</t>
+  </si>
+  <si>
+    <t>DIANJIAN HAIYU LTD FRN 29DEC2049</t>
+  </si>
+  <si>
+    <t>XS1629465797</t>
+  </si>
+  <si>
+    <t>BYXLDX1</t>
+  </si>
+  <si>
+    <t>EASY TACTIC LTD GZRFPR 5 3/4 01/13/22</t>
+  </si>
+  <si>
+    <t>XS1545743442</t>
+  </si>
+  <si>
+    <t>BF5CKX8</t>
+  </si>
+  <si>
+    <t>GEN MOTORS FIN GM 0 06/30/22</t>
+  </si>
+  <si>
+    <t>US37045XBX30</t>
+  </si>
+  <si>
+    <t>B9B31H4</t>
+  </si>
+  <si>
+    <t>GOLDEN EAGLE RET GERGHK 4 5/8 05/21/23</t>
+  </si>
+  <si>
+    <t>USG3958RAB53</t>
+  </si>
+  <si>
+    <t>HESTEEL HONG KON TSSTEE 4 1/4 04/07/20</t>
+  </si>
+  <si>
+    <t>HUARONG FIN II HRAM 4 5/8 06/03/26</t>
+  </si>
+  <si>
+    <t>BYWL2Z7</t>
+  </si>
+  <si>
+    <t>HUARONG FINANCE HRAM 0 04/27/22</t>
+  </si>
+  <si>
+    <t>XS1596795192</t>
+  </si>
+  <si>
     <t>BF04Y37</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>BEIPRO 4.375 03/08/20</t>
+  </si>
+  <si>
+    <t>KEEN IDEA GLB BEIPRO 4 3/8 03/08/20</t>
   </si>
   <si>
     <t>XS1562292026</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>BF08G22</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCAMCL 3 03/09/20</t>
-  </si>
-  <si>
-    <t>XS1573134878</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>BF088D7</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCAMCL 3.65 03/09/22</t>
-  </si>
-  <si>
-    <t>XS1573134522</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>BF04590</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>GRCHAR 6.375 03/07/19 EMTN</t>
-  </si>
-  <si>
-    <t>XS1572352653</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>BF0B212</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>PCPDC 4.75 03/09/22</t>
-  </si>
-  <si>
-    <t>XS1572363858</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>HRAM 5 11/19/25 EMTN</t>
-  </si>
-  <si>
-    <t>CITLTD 3.875 02/28/27 EMTN</t>
-  </si>
-  <si>
-    <t>XS1570263563</t>
-  </si>
-  <si>
-    <t>LENOVO V5.375 PERP EMtn</t>
-  </si>
-  <si>
-    <t>XS1575529539</t>
-  </si>
-  <si>
-    <t>BF0SK86</t>
-  </si>
-  <si>
-    <t>BDC4MV5</t>
-  </si>
-  <si>
-    <t>XS1317967492</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>BD5ZRF4</t>
-  </si>
-  <si>
-    <t>XS1580239207</t>
-  </si>
-  <si>
-    <t>LGEN V5.25 03/21/47 EMTn</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>XS1572322409</t>
-  </si>
-  <si>
-    <t>BCOMFL 4.25 03/21/27 EMTN</t>
-  </si>
-  <si>
-    <t>BF1TMX7</t>
-  </si>
-  <si>
-    <t>BF282K0</t>
-  </si>
-  <si>
-    <t>XS1464929329</t>
-  </si>
-  <si>
-    <t>ROADKG 5 08/09/19</t>
-  </si>
-  <si>
-    <t>BD1FF76</t>
-  </si>
-  <si>
-    <t>XS1565437057</t>
-  </si>
-  <si>
-    <t>FUTLAN 5 02/16/20</t>
-  </si>
-  <si>
-    <t>BDGKNT4</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>BYMZFX8</t>
-  </si>
-  <si>
-    <t>FOSUNI 5.5 08/17/23</t>
-  </si>
-  <si>
-    <t>XS1471856424</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>BDF16K0</t>
-  </si>
-  <si>
-    <t>BD5N6N9</t>
-  </si>
-  <si>
-    <t>GUANGH 7.875 03/30/20</t>
-  </si>
-  <si>
-    <t>XS1581385900</t>
-  </si>
-  <si>
-    <t>HRAM 4.625 06/03/26 EMTN</t>
-  </si>
-  <si>
-    <t>XS1422790615</t>
-  </si>
-  <si>
-    <t>XS1565684062</t>
-  </si>
-  <si>
-    <t>TSSTEE 4.25 04/07/20</t>
-  </si>
-  <si>
-    <t>BYQCMB2</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>ISIN/Geneva</t>
+  </si>
+  <si>
+    <t>BZ0YJN2</t>
+  </si>
+  <si>
+    <t>LOGAN PROPERTY H LOGPH 5 1/4 02/23/23</t>
+  </si>
+  <si>
+    <t>XS1618597535</t>
+  </si>
+  <si>
+    <t>BDFB3Y3</t>
+  </si>
+  <si>
+    <t>MINEJESA CAPITAL BV 4.625% 10AUG2030</t>
+  </si>
+  <si>
+    <t>USN57445AA17</t>
+  </si>
+  <si>
+    <t>BYZMXH6</t>
+  </si>
+  <si>
+    <t>PETROLEOS MEXICANOS FRN 11MAR2022</t>
+  </si>
+  <si>
+    <t>US71656MBN83</t>
+  </si>
+  <si>
+    <t>BYZ6NY5</t>
+  </si>
+  <si>
+    <t>POWERLONG REAL ESTATE 5.95% 19JUL2020</t>
+  </si>
+  <si>
+    <t>XS1645451565</t>
+  </si>
+  <si>
+    <t>RKI FIN 2016 A ROADKG 5 08/09/19</t>
+  </si>
+  <si>
+    <t>BDT74Z5</t>
+  </si>
+  <si>
+    <t>ROYAL BK SCOTLND GRP PLC FRN 15MAY2023</t>
+  </si>
+  <si>
+    <t>US780097BF78</t>
+  </si>
+  <si>
+    <t>BD36XC8</t>
+  </si>
+  <si>
+    <t>SHANDONG ENER AU SHAEGZ 4.55 07/26/20</t>
+  </si>
+  <si>
+    <t>XS1648248455</t>
+  </si>
+  <si>
+    <t>BW9P5P9</t>
+  </si>
+  <si>
+    <t>TIMES PROPERTY TPHL 11.45 03/05/20</t>
+  </si>
+  <si>
+    <t>XS1165129476</t>
+  </si>
+  <si>
+    <t>BZ56SD6</t>
+  </si>
+  <si>
+    <t>US TREASURY N/B T 1 12/31/17</t>
+  </si>
+  <si>
+    <t>US912828N555</t>
   </si>
 </sst>
 </file>
@@ -622,16 +779,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -641,219 +798,425 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="1"/>
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="1"/>
+      <c r="A7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>19</v>
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="1"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="1"/>
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="1"/>
+      <c r="A10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>28</v>
+        <v>12</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="1"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="1" t="s">
-        <v>33</v>
+      <c r="A12" t="s">
+        <v>96</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="1"/>
+        <v>97</v>
+      </c>
+      <c r="C12" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
-        <v>36</v>
+      <c r="A13" t="s">
+        <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="C13" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="1"/>
+        <v>32</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>44</v>
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="1"/>
+        <v>29</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1" t="s">
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1"/>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1"/>
+      <c r="B32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="1"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="1"/>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="1"/>
     </row>
   </sheetData>
+  <sortState ref="A2:C51">
+    <sortCondition ref="A2:A51"/>
+  </sortState>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ver 0.11 logging updated
</commit_message>
<xml_diff>
--- a/samples/InvestmentCodeLookup.xlsx
+++ b/samples/InvestmentCodeLookup.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\citi\samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentManualCount="8"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
   <si>
     <t>CITI code</t>
     <phoneticPr fontId="6" type="noConversion"/>
@@ -346,6 +346,104 @@
   </si>
   <si>
     <t>US912828N555</t>
+  </si>
+  <si>
+    <t>BF04590</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>GRCHAR 6.375 03/07/19 EMTN</t>
+  </si>
+  <si>
+    <t>XS1572352653</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BF0B212</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCPDC 4.75 03/09/22</t>
+  </si>
+  <si>
+    <t>XS1572363858</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BF0SK86</t>
+  </si>
+  <si>
+    <t>CITLTD 3.875 02/28/27 EMTN</t>
+  </si>
+  <si>
+    <t>XS1570263563</t>
+  </si>
+  <si>
+    <t>BDC4MV5</t>
+  </si>
+  <si>
+    <t>LENOVO V5.375 PERP EMtn</t>
+  </si>
+  <si>
+    <t>XS1575529539</t>
+  </si>
+  <si>
+    <t>BD5ZRF4</t>
+  </si>
+  <si>
+    <t>HRAM 5 11/19/25 EMTN</t>
+  </si>
+  <si>
+    <t>XS1317967492</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>BF1TMX7</t>
+  </si>
+  <si>
+    <t>LGEN V5.25 03/21/47 EMTn</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>XS1580239207</t>
+  </si>
+  <si>
+    <t>BF282K0</t>
+  </si>
+  <si>
+    <t>BCOMFL 4.25 03/21/27 EMTN</t>
+  </si>
+  <si>
+    <t>XS1572322409</t>
+  </si>
+  <si>
+    <t>BDGKNT4</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>FUTLAN 5 02/16/20</t>
+  </si>
+  <si>
+    <t>XS1565437057</t>
+  </si>
+  <si>
+    <t>BYMZFX8</t>
+  </si>
+  <si>
+    <t>FOSUNI 5.5 08/17/23</t>
+  </si>
+  <si>
+    <t>XS1471856424</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>BD5N6N9</t>
+  </si>
+  <si>
+    <t>GUANGH 7.875 03/30/20</t>
+  </si>
+  <si>
+    <t>XS1581385900</t>
   </si>
 </sst>
 </file>
@@ -779,10 +877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -884,338 +982,425 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>135</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>136</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="C10" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>14</v>
+      <c r="A11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="C12" t="s">
-        <v>98</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="1" t="s">
-        <v>30</v>
+      <c r="A14" t="s">
+        <v>129</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>32</v>
+        <v>130</v>
+      </c>
+      <c r="C14" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
+        <v>12</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>11</v>
+      <c r="A16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>108</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>109</v>
       </c>
       <c r="C17" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
-        <v>45</v>
+      <c r="A18" t="s">
+        <v>80</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>81</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>69</v>
+      <c r="A19" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" t="s">
-        <v>71</v>
+        <v>31</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>111</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>112</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>102</v>
-      </c>
-      <c r="B22" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22" t="s">
-        <v>104</v>
+      <c r="A22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>26</v>
+      <c r="A23" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>20</v>
+      <c r="A24" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24" t="s">
+        <v>124</v>
+      </c>
+      <c r="C24" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>23</v>
+      <c r="A25" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>44</v>
+      <c r="A26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>6</v>
+      <c r="A27" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="B27" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C28" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+      <c r="B29" t="s">
+        <v>37</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="C30" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" t="s">
-        <v>50</v>
+        <v>24</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>92</v>
-      </c>
-      <c r="B33" t="s">
-        <v>93</v>
-      </c>
-      <c r="C33" t="s">
-        <v>94</v>
+      <c r="A33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>89</v>
-      </c>
-      <c r="B34" t="s">
-        <v>90</v>
-      </c>
-      <c r="C34" t="s">
-        <v>91</v>
+      <c r="A34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
+        <v>132</v>
+      </c>
+      <c r="B35" t="s">
+        <v>133</v>
+      </c>
+      <c r="C35" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
         <v>83</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B45" t="s">
         <v>84</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C45" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
         <v>105</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B46" t="s">
         <v>106</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C46" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="1"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="1"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="1"/>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="1"/>
-    </row>
   </sheetData>
-  <sortState ref="A2:C51">
-    <sortCondition ref="A2:A51"/>
+  <sortState ref="A2:C46">
+    <sortCondition ref="A2:A46"/>
   </sortState>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated citi to ISIN code lookup table. citi code is actually SEDOL code
</commit_message>
<xml_diff>
--- a/samples/InvestmentCodeLookup.xlsx
+++ b/samples/InvestmentCodeLookup.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\citi\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" calcMode="manual" iterate="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="192">
   <si>
     <t>CITI code</t>
     <phoneticPr fontId="6" type="noConversion"/>
@@ -444,6 +444,168 @@
   </si>
   <si>
     <t>XS1581385900</t>
+  </si>
+  <si>
+    <t>BDFB3J8</t>
+  </si>
+  <si>
+    <t>BDGHGJ6</t>
+  </si>
+  <si>
+    <t>BDRVQP3</t>
+  </si>
+  <si>
+    <t>BDZ7S91</t>
+  </si>
+  <si>
+    <t>BD0XWG9</t>
+  </si>
+  <si>
+    <t>BD1FLT0</t>
+  </si>
+  <si>
+    <t>BD3DTT8</t>
+  </si>
+  <si>
+    <t>BD828S2</t>
+  </si>
+  <si>
+    <t>BF04KL7</t>
+  </si>
+  <si>
+    <t>BQR9QX6</t>
+  </si>
+  <si>
+    <t>BVTM092</t>
+  </si>
+  <si>
+    <t>BVYT214</t>
+  </si>
+  <si>
+    <t>BYMT9X8</t>
+  </si>
+  <si>
+    <t>BYQDLW9</t>
+  </si>
+  <si>
+    <t>BYV75N5</t>
+  </si>
+  <si>
+    <t>BYWYTF5</t>
+  </si>
+  <si>
+    <t>BYW5T14</t>
+  </si>
+  <si>
+    <t>BYXBGB0</t>
+  </si>
+  <si>
+    <t>EHICAR 5 7/8 08/14/22</t>
+  </si>
+  <si>
+    <t>CHALUM 4 08/25/21</t>
+  </si>
+  <si>
+    <t>TPHL 6 1/4 01/23/20</t>
+  </si>
+  <si>
+    <t>COGARD 4 3/4 07/25/22</t>
+  </si>
+  <si>
+    <t>RUYIGR 7 1/2 12/19/19</t>
+  </si>
+  <si>
+    <t>UBS 7 1/8 PERP</t>
+  </si>
+  <si>
+    <t>EVERRE 7 03/23/20</t>
+  </si>
+  <si>
+    <t>CHALUM 4 1/4 PERP</t>
+  </si>
+  <si>
+    <t>XINHUZ 6 03/01/20</t>
+  </si>
+  <si>
+    <t>WESCHI 6 1/2 09/11/19</t>
+  </si>
+  <si>
+    <t>CARINC 6 1/8 02/04/20</t>
+  </si>
+  <si>
+    <t>AGILE 9 05/21/20</t>
+  </si>
+  <si>
+    <t>CIFIHG 7 3/4 06/05/20</t>
+  </si>
+  <si>
+    <t>CNBG 4 3/8 PERP</t>
+  </si>
+  <si>
+    <t>YZCOAL 5 3/4 PERP</t>
+  </si>
+  <si>
+    <t>HRAM 4 1/2 PERP</t>
+  </si>
+  <si>
+    <t>KAISAG 7 7/8 06/30/21</t>
+  </si>
+  <si>
+    <t>CHINSC 5 7/8 03/10/22</t>
+  </si>
+  <si>
+    <t>XS1657420441</t>
+  </si>
+  <si>
+    <t>XS1449592051</t>
+  </si>
+  <si>
+    <t>XS1549245238</t>
+  </si>
+  <si>
+    <t>XS1637076164</t>
+  </si>
+  <si>
+    <t>XS1523057021</t>
+  </si>
+  <si>
+    <t>CH0331455318</t>
+  </si>
+  <si>
+    <t>XS1580430681</t>
+  </si>
+  <si>
+    <t>XS1511610906</t>
+  </si>
+  <si>
+    <t>XS1560668425</t>
+  </si>
+  <si>
+    <t>XS1107316041</t>
+  </si>
+  <si>
+    <t>XS1163232900</t>
+  </si>
+  <si>
+    <t>XS1215617272</t>
+  </si>
+  <si>
+    <t>XS1160444391</t>
+  </si>
+  <si>
+    <t>XS1334043095</t>
+  </si>
+  <si>
+    <t>XS1577730895</t>
+  </si>
+  <si>
+    <t>XS1555076162</t>
+  </si>
+  <si>
+    <t>XS1627597286</t>
+  </si>
+  <si>
+    <t>XS1575984734</t>
   </si>
 </sst>
 </file>
@@ -551,7 +713,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -569,6 +731,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -877,10 +1040,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47:C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1396,6 +1559,204 @@
       </c>
       <c r="C46" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated mapping from SEDOL to ISIN
</commit_message>
<xml_diff>
--- a/samples/InvestmentCodeLookup.xlsx
+++ b/samples/InvestmentCodeLookup.xlsx
@@ -16,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" calcMode="manual" iterate="1"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="204">
   <si>
     <t>CITI code</t>
     <phoneticPr fontId="6" type="noConversion"/>
@@ -606,6 +606,42 @@
   </si>
   <si>
     <t>XS1575984734</t>
+  </si>
+  <si>
+    <t>BDDWMY1</t>
+  </si>
+  <si>
+    <t>BDTYZ31</t>
+  </si>
+  <si>
+    <t>BF07339</t>
+  </si>
+  <si>
+    <t>SOPOWZ 3 1/2 05/08/27</t>
+  </si>
+  <si>
+    <t>LOGPH 5 3/4 01/03/22</t>
+  </si>
+  <si>
+    <t>CHJMAO 4 PERP</t>
+  </si>
+  <si>
+    <t>USG2120QAC09</t>
+  </si>
+  <si>
+    <t>XS1541978851</t>
+  </si>
+  <si>
+    <t>XS1673588452</t>
+  </si>
+  <si>
+    <t>BYW5T25</t>
+  </si>
+  <si>
+    <t>KAISAG 8 1/2 06/30/22</t>
+  </si>
+  <si>
+    <t>XS1627597955</t>
   </si>
 </sst>
 </file>
@@ -1040,10 +1076,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1757,6 +1793,50 @@
       </c>
       <c r="C64" s="9" t="s">
         <v>191</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="B65" t="s">
+        <v>195</v>
+      </c>
+      <c r="C65" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="B66" t="s">
+        <v>196</v>
+      </c>
+      <c r="C66" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B67" t="s">
+        <v>197</v>
+      </c>
+      <c r="C67" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update SEDOL - ISIN mapping
</commit_message>
<xml_diff>
--- a/samples/InvestmentCodeLookup.xlsx
+++ b/samples/InvestmentCodeLookup.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -16,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="237">
   <si>
     <t>CITI code</t>
     <phoneticPr fontId="6" type="noConversion"/>
@@ -642,12 +642,111 @@
   </si>
   <si>
     <t>XS1627597955</t>
+  </si>
+  <si>
+    <t>BD02SL3</t>
+  </si>
+  <si>
+    <t>BD5DB45</t>
+  </si>
+  <si>
+    <t>BD878G5</t>
+  </si>
+  <si>
+    <t>BD96452</t>
+  </si>
+  <si>
+    <t>BF42H16</t>
+  </si>
+  <si>
+    <t>BF5V950</t>
+  </si>
+  <si>
+    <t>BSKPG02</t>
+  </si>
+  <si>
+    <t>BTC0J70</t>
+  </si>
+  <si>
+    <t>BYWK351</t>
+  </si>
+  <si>
+    <t>BZ0X456</t>
+  </si>
+  <si>
+    <t>BZ4FBY6</t>
+  </si>
+  <si>
+    <t>AGRBK 0 05/16/19</t>
+  </si>
+  <si>
+    <t>ICBCAS 0 02/21/22</t>
+  </si>
+  <si>
+    <t>MEXCAT 4 1/4 10/31/26</t>
+  </si>
+  <si>
+    <t>OCTOWN 4.3 PERP</t>
+  </si>
+  <si>
+    <t>HAOHUA 3 1/2 07/19/22</t>
+  </si>
+  <si>
+    <t>SUNAC 6 7/8 08/08/20</t>
+  </si>
+  <si>
+    <t>BCHINA 5 11/13/24</t>
+  </si>
+  <si>
+    <t>ICBCAS 6 PERP</t>
+  </si>
+  <si>
+    <t>VNET 7 08/17/20</t>
+  </si>
+  <si>
+    <t>BCHINA 0 04/20/20</t>
+  </si>
+  <si>
+    <t>BCHINA 0 05/11/20</t>
+  </si>
+  <si>
+    <t>XS1411380220</t>
+  </si>
+  <si>
+    <t>XS1566971252</t>
+  </si>
+  <si>
+    <t>USP6629MAA01</t>
+  </si>
+  <si>
+    <t>XS1692254359</t>
+  </si>
+  <si>
+    <t>XS1644429695</t>
+  </si>
+  <si>
+    <t>XS1594400100</t>
+  </si>
+  <si>
+    <t>US06120TAA60</t>
+  </si>
+  <si>
+    <t>USY39656AA40</t>
+  </si>
+  <si>
+    <t>XS1692589028</t>
+  </si>
+  <si>
+    <t>XS1599275713</t>
+  </si>
+  <si>
+    <t>XS1608002082</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -865,6 +964,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -900,6 +1016,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1076,10 +1209,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69:C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1837,6 +1970,127 @@
       </c>
       <c r="C68" s="9" t="s">
         <v>203</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>